<commit_message>
Switch Statement and Gantt Chart
Started making the switch statement for the stepper motor, started making the counter for the motor revolution, and finally made adjustments to the Gantt Chart.
</commit_message>
<xml_diff>
--- a/Automated_Smart_Blinds_Gantt_Chart.xlsx
+++ b/Automated_Smart_Blinds_Gantt_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revster13\Documents\CST 371 &amp; 372\JP\AutomatedSmartBlinds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5B6C92-46F5-4936-8AED-F7029E25CFF8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34C98C-F56C-4EC4-9908-1D35118B4AF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1357,8 +1357,8 @@
   <dimension ref="A1:BO69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -2304,13 +2304,13 @@
         <v>38</v>
       </c>
       <c r="C31" s="21">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D31" s="21">
         <v>1</v>
       </c>
       <c r="E31" s="21">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F31" s="21">
         <v>0</v>
@@ -2324,7 +2324,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="21">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D32" s="21">
         <v>1</v>
@@ -2344,7 +2344,7 @@
         <v>40</v>
       </c>
       <c r="C33" s="21">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D33" s="21">
         <v>1</v>
@@ -2364,7 +2364,7 @@
         <v>41</v>
       </c>
       <c r="C34" s="21">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D34" s="21">
         <v>1</v>
@@ -2384,13 +2384,13 @@
         <v>42</v>
       </c>
       <c r="C35" s="21">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D35" s="21">
         <v>1</v>
       </c>
       <c r="E35" s="21">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F35" s="21">
         <v>1</v>
@@ -2404,7 +2404,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="21">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D36" s="21">
         <v>1</v>
@@ -2424,7 +2424,7 @@
         <v>44</v>
       </c>
       <c r="C37" s="21">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D37" s="21">
         <v>1</v>
@@ -2444,7 +2444,7 @@
         <v>45</v>
       </c>
       <c r="C38" s="21">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D38" s="21">
         <v>2</v>
@@ -2464,13 +2464,13 @@
         <v>46</v>
       </c>
       <c r="C39" s="21">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D39" s="21">
         <v>1</v>
       </c>
       <c r="E39" s="21">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F39" s="21">
         <v>0</v>
@@ -2484,7 +2484,7 @@
         <v>47</v>
       </c>
       <c r="C40" s="21">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D40" s="21">
         <v>1</v>
@@ -2504,7 +2504,7 @@
         <v>48</v>
       </c>
       <c r="C41" s="21">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D41" s="21">
         <v>1</v>
@@ -2524,13 +2524,13 @@
         <v>49</v>
       </c>
       <c r="C42" s="21">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D42" s="21">
         <v>1</v>
       </c>
       <c r="E42" s="21">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F42" s="21">
         <v>1</v>
@@ -2544,7 +2544,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="21">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D43" s="21">
         <v>1</v>
@@ -2564,7 +2564,7 @@
         <v>51</v>
       </c>
       <c r="C44" s="21">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D44" s="21">
         <v>1</v>
@@ -2584,7 +2584,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="21">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D45" s="21">
         <v>1</v>

</xml_diff>